<commit_message>
Incorporación de nombres elecciones a clase Tablero
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA95FC9D-8C89-C04D-BDF3-D9BA2EBA287B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9060360-3A46-4140-A736-53306296C731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
+    <workbookView xWindow="-24420" yWindow="-80" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nombre</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>#606c38</t>
+  </si>
+  <si>
+    <t>Gobernatura 17</t>
+  </si>
+  <si>
+    <t>gb_17</t>
+  </si>
+  <si>
+    <t>#dda15e</t>
   </si>
 </sst>
 </file>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,78 +489,89 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nuevos colores y elecciones en archivos data
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9060360-3A46-4140-A736-53306296C731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D57637-92EB-4B4E-A572-5983FFCB4268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24420" yWindow="-80" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
+    <workbookView xWindow="-28800" yWindow="-80" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Nombre</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>#dda15e</t>
+  </si>
+  <si>
+    <t>Presidencia Municipal 15</t>
+  </si>
+  <si>
+    <t>pm_15</t>
+  </si>
+  <si>
+    <t>#669bbc</t>
   </si>
 </sst>
 </file>
@@ -468,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,89 +498,100 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección de clase y actualización de nombres_elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D57637-92EB-4B4E-A572-5983FFCB4268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3402D6EE-7D1D-A04D-A6E5-E040E04F8276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="-80" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Nombre</t>
   </si>
@@ -126,6 +126,24 @@
   </si>
   <si>
     <t>#669bbc</t>
+  </si>
+  <si>
+    <t>Gobernatura 23</t>
+  </si>
+  <si>
+    <t>gb_23</t>
+  </si>
+  <si>
+    <t>#283618</t>
+  </si>
+  <si>
+    <t>Senado 18</t>
+  </si>
+  <si>
+    <t>sen_18</t>
+  </si>
+  <si>
+    <t>348cae4</t>
   </si>
 </sst>
 </file>
@@ -477,13 +495,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -564,35 +585,57 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporación de presidencia 2018 en rda para de nombres de elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3402D6EE-7D1D-A04D-A6E5-E040E04F8276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D888906-E0A0-9A45-8466-9CDC2E40F60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-80" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Nombre</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>348cae4</t>
+  </si>
+  <si>
+    <t>Presidencia 18</t>
+  </si>
+  <si>
+    <t>pr_18</t>
+  </si>
+  <si>
+    <t>#57cc99</t>
   </si>
 </sst>
 </file>
@@ -495,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,100 +550,111 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incorporación del distrito federal 2015 en xlsx nombre_elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D888906-E0A0-9A45-8466-9CDC2E40F60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B9004E-D2DD-6740-AA75-CACB5D544B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Nombre</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>#57cc99</t>
+  </si>
+  <si>
+    <t>Distrito federal 15</t>
+  </si>
+  <si>
+    <t>df_15</t>
+  </si>
+  <si>
+    <t>#ffc8dd</t>
   </si>
 </sst>
 </file>
@@ -504,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,122 +548,133 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusión de nuevos nombre de elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B9004E-D2DD-6740-AA75-CACB5D544B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66B0865-34D9-E54A-B2BB-C86872C048DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Nombre</t>
   </si>
@@ -143,9 +143,6 @@
     <t>sen_18</t>
   </si>
   <si>
-    <t>348cae4</t>
-  </si>
-  <si>
     <t>Presidencia 18</t>
   </si>
   <si>
@@ -162,6 +159,36 @@
   </si>
   <si>
     <t>#ffc8dd</t>
+  </si>
+  <si>
+    <t>Gobernatura 19</t>
+  </si>
+  <si>
+    <t>gb_19</t>
+  </si>
+  <si>
+    <t>#348cae4</t>
+  </si>
+  <si>
+    <t>Distrito local 19</t>
+  </si>
+  <si>
+    <t>dl_19</t>
+  </si>
+  <si>
+    <t>#5a189a</t>
+  </si>
+  <si>
+    <t>#6b9080</t>
+  </si>
+  <si>
+    <t>Presidencia Municipal 19</t>
+  </si>
+  <si>
+    <t>pm_19</t>
+  </si>
+  <si>
+    <t>#d68c45</t>
   </si>
 </sst>
 </file>
@@ -513,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,13 +575,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -570,13 +597,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -631,50 +658,83 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusión de gb_21 en nombres_elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66B0865-34D9-E54A-B2BB-C86872C048DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B936405F-7DAF-7844-BE29-A6671373B78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Nombre</t>
   </si>
@@ -167,9 +167,6 @@
     <t>gb_19</t>
   </si>
   <si>
-    <t>#348cae4</t>
-  </si>
-  <si>
     <t>Distrito local 19</t>
   </si>
   <si>
@@ -189,6 +186,18 @@
   </si>
   <si>
     <t>#d68c45</t>
+  </si>
+  <si>
+    <t>#348cae</t>
+  </si>
+  <si>
+    <t>Gobernatura 21</t>
+  </si>
+  <si>
+    <t>gb_21</t>
+  </si>
+  <si>
+    <t>#4361ee</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,18 +667,18 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -680,18 +689,18 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -707,34 +716,45 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección de geompointrange e inclusión de gb_21 en nombres_elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66B0865-34D9-E54A-B2BB-C86872C048DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0343BB-F1DD-2340-81AD-2A6FC1EB3EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Nombre</t>
   </si>
@@ -167,9 +167,6 @@
     <t>gb_19</t>
   </si>
   <si>
-    <t>#348cae4</t>
-  </si>
-  <si>
     <t>Distrito local 19</t>
   </si>
   <si>
@@ -189,6 +186,18 @@
   </si>
   <si>
     <t>#d68c45</t>
+  </si>
+  <si>
+    <t>#348cae</t>
+  </si>
+  <si>
+    <t>Gobernatura 21</t>
+  </si>
+  <si>
+    <t>gb_21</t>
+  </si>
+  <si>
+    <t>#588157</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,18 +667,18 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -680,18 +689,18 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -707,34 +716,45 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incorporación de pr 06 y pr 12 a nombres elecciones
</commit_message>
<xml_diff>
--- a/data-raw/nombres_elecciones.xlsx
+++ b/data-raw/nombres_elecciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaellopez/Documents/Git/aelectoral2/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B936405F-7DAF-7844-BE29-A6671373B78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BCDB65-E724-AC44-9447-BFE129EA56B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{F81083C0-5398-8C47-8510-82DDE0B61B4C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Nombre</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>#4361ee</t>
+  </si>
+  <si>
+    <t>Presidencia 12</t>
+  </si>
+  <si>
+    <t>pr_12</t>
+  </si>
+  <si>
+    <t>#d6ccc2</t>
+  </si>
+  <si>
+    <t>Presidencia 06</t>
+  </si>
+  <si>
+    <t>pr_06</t>
+  </si>
+  <si>
+    <t>#b5838d</t>
   </si>
 </sst>
 </file>
@@ -549,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A5188D9-48EB-4D4B-8F48-598BF43CF274}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,188 +591,210 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>